<commit_message>
check year and file translation
</commit_message>
<xml_diff>
--- a/public/translation/ArabTranslate.xlsx
+++ b/public/translation/ArabTranslate.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bailsan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="English_File__1_translated" localSheetId="0">Sheet1!$A$1:$F$324</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="688">
   <si>
     <t>year</t>
   </si>
@@ -2102,12 +2102,18 @@
   </si>
   <si>
     <t>لا يوجد مدرسين</t>
+  </si>
+  <si>
+    <t>msg_bbb</t>
+  </si>
+  <si>
+    <t>ملحوظة سوف يتم غلق المحاضرة في حالة عدم دخول احد خلال ٥ دقائق من وقت بداية المحاضرة</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2448,21 +2454,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C355"/>
+  <dimension ref="A1:C356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="C355" sqref="C355"/>
+    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>613</v>
       </c>
@@ -2473,7 +2479,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2528,7 +2534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2539,7 +2545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2550,7 +2556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2616,7 +2622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2627,7 +2633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2649,7 +2655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2682,7 +2688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2704,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2715,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2748,7 +2754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -2792,7 +2798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2803,7 +2809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -2814,7 +2820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2825,7 +2831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -2902,7 +2908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -2946,7 +2952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2957,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -2979,7 +2985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -3012,7 +3018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -3023,7 +3029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>617</v>
       </c>
@@ -3034,7 +3040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -3045,7 +3051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -3056,7 +3062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -3078,7 +3084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>108</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -3111,7 +3117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>114</v>
       </c>
@@ -3122,7 +3128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>116</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>118</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>120</v>
       </c>
@@ -3155,7 +3161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>122</v>
       </c>
@@ -3166,7 +3172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -3177,7 +3183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>128</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>130</v>
       </c>
@@ -3210,7 +3216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>132</v>
       </c>
@@ -3221,7 +3227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>134</v>
       </c>
@@ -3232,7 +3238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>136</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>138</v>
       </c>
@@ -3254,7 +3260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="b">
         <v>1</v>
       </c>
@@ -3287,7 +3293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="b">
         <v>0</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -3309,7 +3315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>148</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>150</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>152</v>
       </c>
@@ -3342,7 +3348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>154</v>
       </c>
@@ -3353,7 +3359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>156</v>
       </c>
@@ -3364,7 +3370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>158</v>
       </c>
@@ -3375,7 +3381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>159</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>161</v>
       </c>
@@ -3397,7 +3403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>163</v>
       </c>
@@ -3408,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>165</v>
       </c>
@@ -3419,7 +3425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>167</v>
       </c>
@@ -3430,7 +3436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>169</v>
       </c>
@@ -3441,7 +3447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>171</v>
       </c>
@@ -3452,7 +3458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>173</v>
       </c>
@@ -3463,7 +3469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>175</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>177</v>
       </c>
@@ -3485,7 +3491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>179</v>
       </c>
@@ -3496,7 +3502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>181</v>
       </c>
@@ -3507,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -3518,7 +3524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>185</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>187</v>
       </c>
@@ -3540,7 +3546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>189</v>
       </c>
@@ -3551,7 +3557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>191</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>193</v>
       </c>
@@ -3573,7 +3579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>195</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>197</v>
       </c>
@@ -3595,7 +3601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>199</v>
       </c>
@@ -3606,7 +3612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>201</v>
       </c>
@@ -3617,7 +3623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>203</v>
       </c>
@@ -3628,7 +3634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>205</v>
       </c>
@@ -3639,7 +3645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>207</v>
       </c>
@@ -3650,7 +3656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>209</v>
       </c>
@@ -3661,7 +3667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>211</v>
       </c>
@@ -3672,7 +3678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>213</v>
       </c>
@@ -3683,7 +3689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>215</v>
       </c>
@@ -3694,7 +3700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>217</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>219</v>
       </c>
@@ -3716,7 +3722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>221</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>223</v>
       </c>
@@ -3738,7 +3744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>225</v>
       </c>
@@ -3749,7 +3755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>226</v>
       </c>
@@ -3760,7 +3766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>227</v>
       </c>
@@ -3771,7 +3777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>229</v>
       </c>
@@ -3782,7 +3788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>231</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>233</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>235</v>
       </c>
@@ -3815,7 +3821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>237</v>
       </c>
@@ -3826,7 +3832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>239</v>
       </c>
@@ -3837,7 +3843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>241</v>
       </c>
@@ -3848,7 +3854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>243</v>
       </c>
@@ -3859,7 +3865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>245</v>
       </c>
@@ -3870,7 +3876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>247</v>
       </c>
@@ -3881,7 +3887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>248</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>249</v>
       </c>
@@ -3903,7 +3909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>251</v>
       </c>
@@ -3914,7 +3920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>253</v>
       </c>
@@ -3925,7 +3931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>255</v>
       </c>
@@ -3936,7 +3942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>257</v>
       </c>
@@ -3947,7 +3953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>259</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>260</v>
       </c>
@@ -3969,7 +3975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>261</v>
       </c>
@@ -3980,7 +3986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>262</v>
       </c>
@@ -3991,7 +3997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>263</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>264</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>266</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>268</v>
       </c>
@@ -4035,7 +4041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>270</v>
       </c>
@@ -4046,7 +4052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>272</v>
       </c>
@@ -4057,7 +4063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>274</v>
       </c>
@@ -4068,7 +4074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>276</v>
       </c>
@@ -4079,7 +4085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>278</v>
       </c>
@@ -4090,7 +4096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>280</v>
       </c>
@@ -4101,7 +4107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>282</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>284</v>
       </c>
@@ -4123,7 +4129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>286</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>288</v>
       </c>
@@ -4145,7 +4151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>290</v>
       </c>
@@ -4156,7 +4162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>292</v>
       </c>
@@ -4167,7 +4173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>294</v>
       </c>
@@ -4178,7 +4184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>296</v>
       </c>
@@ -4189,7 +4195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>298</v>
       </c>
@@ -4200,7 +4206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>300</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>302</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>304</v>
       </c>
@@ -4233,7 +4239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>306</v>
       </c>
@@ -4244,7 +4250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>308</v>
       </c>
@@ -4255,7 +4261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>310</v>
       </c>
@@ -4266,7 +4272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>312</v>
       </c>
@@ -4277,7 +4283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>314</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>316</v>
       </c>
@@ -4299,7 +4305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>318</v>
       </c>
@@ -4310,7 +4316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>320</v>
       </c>
@@ -4321,7 +4327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>322</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>324</v>
       </c>
@@ -4343,7 +4349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>326</v>
       </c>
@@ -4354,7 +4360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>328</v>
       </c>
@@ -4365,7 +4371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>330</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>332</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>334</v>
       </c>
@@ -4398,7 +4404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>336</v>
       </c>
@@ -4409,7 +4415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>338</v>
       </c>
@@ -4420,7 +4426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>340</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>341</v>
       </c>
@@ -4442,7 +4448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>343</v>
       </c>
@@ -4453,7 +4459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>344</v>
       </c>
@@ -4464,7 +4470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>346</v>
       </c>
@@ -4475,7 +4481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>347</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>349</v>
       </c>
@@ -4497,7 +4503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>351</v>
       </c>
@@ -4508,7 +4514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>353</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>354</v>
       </c>
@@ -4530,7 +4536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>356</v>
       </c>
@@ -4541,7 +4547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>358</v>
       </c>
@@ -4552,7 +4558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>360</v>
       </c>
@@ -4563,7 +4569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>362</v>
       </c>
@@ -4574,7 +4580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>364</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>366</v>
       </c>
@@ -4596,7 +4602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>368</v>
       </c>
@@ -4607,7 +4613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>370</v>
       </c>
@@ -4618,7 +4624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>372</v>
       </c>
@@ -4629,7 +4635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>374</v>
       </c>
@@ -4640,7 +4646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>376</v>
       </c>
@@ -4651,7 +4657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>378</v>
       </c>
@@ -4662,7 +4668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>380</v>
       </c>
@@ -4673,7 +4679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>382</v>
       </c>
@@ -4684,7 +4690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>384</v>
       </c>
@@ -4695,7 +4701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>386</v>
       </c>
@@ -4706,7 +4712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>388</v>
       </c>
@@ -4717,7 +4723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>390</v>
       </c>
@@ -4728,7 +4734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>392</v>
       </c>
@@ -4739,7 +4745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>394</v>
       </c>
@@ -4750,7 +4756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>396</v>
       </c>
@@ -4761,7 +4767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>398</v>
       </c>
@@ -4772,7 +4778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>400</v>
       </c>
@@ -4783,7 +4789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>402</v>
       </c>
@@ -4794,7 +4800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>404</v>
       </c>
@@ -4805,7 +4811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>406</v>
       </c>
@@ -4816,7 +4822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>408</v>
       </c>
@@ -4827,7 +4833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>410</v>
       </c>
@@ -4838,7 +4844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>412</v>
       </c>
@@ -4849,7 +4855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>414</v>
       </c>
@@ -4860,7 +4866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>416</v>
       </c>
@@ -4871,7 +4877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>418</v>
       </c>
@@ -4882,7 +4888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>420</v>
       </c>
@@ -4893,7 +4899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>422</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>424</v>
       </c>
@@ -4915,7 +4921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>426</v>
       </c>
@@ -4926,7 +4932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>428</v>
       </c>
@@ -4937,7 +4943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>430</v>
       </c>
@@ -4948,7 +4954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>432</v>
       </c>
@@ -4959,7 +4965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>434</v>
       </c>
@@ -4970,7 +4976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>436</v>
       </c>
@@ -4981,7 +4987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>438</v>
       </c>
@@ -4992,7 +4998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>440</v>
       </c>
@@ -5003,7 +5009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>441</v>
       </c>
@@ -5014,7 +5020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>443</v>
       </c>
@@ -5025,7 +5031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>445</v>
       </c>
@@ -5036,7 +5042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>447</v>
       </c>
@@ -5047,7 +5053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>449</v>
       </c>
@@ -5058,7 +5064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>451</v>
       </c>
@@ -5069,7 +5075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>453</v>
       </c>
@@ -5080,7 +5086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>455</v>
       </c>
@@ -5091,7 +5097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>457</v>
       </c>
@@ -5102,7 +5108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>459</v>
       </c>
@@ -5113,7 +5119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>461</v>
       </c>
@@ -5124,7 +5130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>462</v>
       </c>
@@ -5135,7 +5141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>464</v>
       </c>
@@ -5146,7 +5152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>466</v>
       </c>
@@ -5157,7 +5163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>468</v>
       </c>
@@ -5168,7 +5174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>470</v>
       </c>
@@ -5179,7 +5185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>472</v>
       </c>
@@ -5190,7 +5196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>474</v>
       </c>
@@ -5201,7 +5207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>476</v>
       </c>
@@ -5212,7 +5218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>478</v>
       </c>
@@ -5223,7 +5229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>480</v>
       </c>
@@ -5234,7 +5240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>482</v>
       </c>
@@ -5245,7 +5251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>484</v>
       </c>
@@ -5256,7 +5262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>486</v>
       </c>
@@ -5267,7 +5273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>487</v>
       </c>
@@ -5278,7 +5284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>489</v>
       </c>
@@ -5289,7 +5295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>491</v>
       </c>
@@ -5300,7 +5306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>493</v>
       </c>
@@ -5311,7 +5317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>495</v>
       </c>
@@ -5322,7 +5328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>497</v>
       </c>
@@ -5333,7 +5339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>499</v>
       </c>
@@ -5344,7 +5350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>501</v>
       </c>
@@ -5355,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>503</v>
       </c>
@@ -5366,7 +5372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>505</v>
       </c>
@@ -5377,7 +5383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>507</v>
       </c>
@@ -5388,7 +5394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>509</v>
       </c>
@@ -5399,7 +5405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>511</v>
       </c>
@@ -5410,7 +5416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>513</v>
       </c>
@@ -5421,7 +5427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>515</v>
       </c>
@@ -5432,7 +5438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>517</v>
       </c>
@@ -5443,7 +5449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>519</v>
       </c>
@@ -5454,7 +5460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>521</v>
       </c>
@@ -5465,7 +5471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>523</v>
       </c>
@@ -5476,7 +5482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>525</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>527</v>
       </c>
@@ -5498,7 +5504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>529</v>
       </c>
@@ -5509,7 +5515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>531</v>
       </c>
@@ -5520,7 +5526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>532</v>
       </c>
@@ -5531,7 +5537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>534</v>
       </c>
@@ -5542,7 +5548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>536</v>
       </c>
@@ -5553,7 +5559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>538</v>
       </c>
@@ -5564,7 +5570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>540</v>
       </c>
@@ -5575,7 +5581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>542</v>
       </c>
@@ -5586,7 +5592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>544</v>
       </c>
@@ -5597,7 +5603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>546</v>
       </c>
@@ -5608,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>548</v>
       </c>
@@ -5619,7 +5625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>550</v>
       </c>
@@ -5630,7 +5636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>552</v>
       </c>
@@ -5641,7 +5647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>554</v>
       </c>
@@ -5652,7 +5658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>556</v>
       </c>
@@ -5663,7 +5669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>558</v>
       </c>
@@ -5674,7 +5680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>559</v>
       </c>
@@ -5685,7 +5691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>561</v>
       </c>
@@ -5696,7 +5702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>563</v>
       </c>
@@ -5707,7 +5713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>565</v>
       </c>
@@ -5718,7 +5724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>567</v>
       </c>
@@ -5729,7 +5735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>568</v>
       </c>
@@ -5740,7 +5746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>569</v>
       </c>
@@ -5751,7 +5757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>570</v>
       </c>
@@ -5762,7 +5768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>572</v>
       </c>
@@ -5773,7 +5779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>574</v>
       </c>
@@ -5784,7 +5790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>576</v>
       </c>
@@ -5795,7 +5801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>578</v>
       </c>
@@ -5806,7 +5812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>580</v>
       </c>
@@ -5817,7 +5823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>582</v>
       </c>
@@ -5828,7 +5834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>584</v>
       </c>
@@ -5839,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>586</v>
       </c>
@@ -5850,7 +5856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>588</v>
       </c>
@@ -5861,7 +5867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>590</v>
       </c>
@@ -5872,7 +5878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>592</v>
       </c>
@@ -5883,7 +5889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>594</v>
       </c>
@@ -5894,7 +5900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>596</v>
       </c>
@@ -5905,7 +5911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>598</v>
       </c>
@@ -5916,7 +5922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>600</v>
       </c>
@@ -5927,7 +5933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>601</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>603</v>
       </c>
@@ -5949,7 +5955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>605</v>
       </c>
@@ -5960,7 +5966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>607</v>
       </c>
@@ -5971,7 +5977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>608</v>
       </c>
@@ -5982,7 +5988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>618</v>
       </c>
@@ -5993,7 +5999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>620</v>
       </c>
@@ -6004,7 +6010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>623</v>
       </c>
@@ -6015,7 +6021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>625</v>
       </c>
@@ -6026,7 +6032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>627</v>
       </c>
@@ -6037,7 +6043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>629</v>
       </c>
@@ -6048,7 +6054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>670</v>
       </c>
@@ -6059,7 +6065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>632</v>
       </c>
@@ -6070,7 +6076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>634</v>
       </c>
@@ -6081,7 +6087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>636</v>
       </c>
@@ -6092,7 +6098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>640</v>
       </c>
@@ -6103,7 +6109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>641</v>
       </c>
@@ -6114,7 +6120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>643</v>
       </c>
@@ -6125,7 +6131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>645</v>
       </c>
@@ -6136,7 +6142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>647</v>
       </c>
@@ -6147,7 +6153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>648</v>
       </c>
@@ -6158,7 +6164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>651</v>
       </c>
@@ -6169,7 +6175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>0</v>
       </c>
@@ -6180,7 +6186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>1</v>
       </c>
@@ -6191,7 +6197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>653</v>
       </c>
@@ -6202,7 +6208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>655</v>
       </c>
@@ -6213,7 +6219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>658</v>
       </c>
@@ -6224,7 +6230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>660</v>
       </c>
@@ -6235,7 +6241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>662</v>
       </c>
@@ -6246,7 +6252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>664</v>
       </c>
@@ -6257,7 +6263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>666</v>
       </c>
@@ -6268,7 +6274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>668</v>
       </c>
@@ -6279,7 +6285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>672</v>
       </c>
@@ -6290,7 +6296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A349" s="2" t="s">
         <v>674</v>
       </c>
@@ -6301,7 +6307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B350" t="s">
         <v>676</v>
       </c>
@@ -6309,7 +6315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>677</v>
       </c>
@@ -6320,7 +6326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>679</v>
       </c>
@@ -6331,7 +6337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>681</v>
       </c>
@@ -6342,7 +6348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>91</v>
       </c>
@@ -6353,7 +6359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355" s="3" t="s">
         <v>684</v>
       </c>
@@ -6361,6 +6367,17 @@
         <v>685</v>
       </c>
       <c r="C355">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>686</v>
+      </c>
+      <c r="B356" t="s">
+        <v>687</v>
+      </c>
+      <c r="C356">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new translation sheets again
</commit_message>
<xml_diff>
--- a/public/translation/ArabTranslate.xlsx
+++ b/public/translation/ArabTranslate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B2C648-3C6E-4C0A-8AA5-E7DCE9410D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6E709E-1664-4BAA-8D37-BD9B4D1B94D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="799">
   <si>
     <t>year</t>
   </si>
@@ -2427,6 +2427,21 @@
   </si>
   <si>
     <t>إعلان</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>تسجيلات</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>please_select_course_and_class</t>
+  </si>
+  <si>
+    <t>من فضلك إختار الفصل و المادة</t>
   </si>
 </sst>
 </file>
@@ -2781,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C411"/>
+  <dimension ref="A1:C414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="B410" sqref="B410"/>
+    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
+      <selection activeCell="A414" sqref="A414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7313,6 +7328,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="412" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A412" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="B412" s="11" t="s">
+        <v>795</v>
+      </c>
+      <c r="C412" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A413" s="11" t="s">
+        <v>796</v>
+      </c>
+      <c r="B413" s="11" t="s">
+        <v>767</v>
+      </c>
+      <c r="C413" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A414" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="B414" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="C414" s="11">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>